<commit_message>
Agrego reporte de bugs
</commit_message>
<xml_diff>
--- a/bugs/reporte_bugs.xlsx.xlsx
+++ b/bugs/reporte_bugs.xlsx.xlsx
@@ -1,57 +1,187 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ProyectoFinal\ProyectoFinal-Nerea\bugs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E39FB7-8503-48D0-B4A7-0E25F10932CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="173" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId5"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+  <si>
+    <t>Título Descriptivo</t>
+  </si>
+  <si>
+    <t>Pasos para reproducir</t>
+  </si>
+  <si>
+    <t>Resultado esperado vs obtenido</t>
+  </si>
+  <si>
+    <t>Severidad</t>
+  </si>
+  <si>
+    <t>Evidencia visual</t>
+  </si>
+  <si>
+    <t>Intentos ilimitados de inicio de sesión con contraseña inválida</t>
+  </si>
+  <si>
+    <t>1.Abrir app.
+2.Ir a la pantalla “Iniciar sesión”.
+3.Ingresar un usuario válido y contraseña incorrecta.
+4.Repetir el intento más de 5 veces consecutivas.</t>
+  </si>
+  <si>
+    <t>Resultado esperado: La cuenta debería bloquearse temporalmente o mostrar un mensaje indicando límite de intentos alcanzado.
+Resultado obtenido: La aplicación permite continuar intentando iniciar sesión sin ningún tipo de restricción o bloqueo</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>El posteo no se cancela al perder conexión a internet (modo avión)</t>
+  </si>
+  <si>
+    <t>1.Abrir app.
+2.Activar “Modo avión” en el dispositivo.
+3.Intentar publicar una imagen.
+4.Confirmar el envío.</t>
+  </si>
+  <si>
+    <t>Resultado esperado: La aplicación debería cancelar el posteo automáticamente o mostrar un mensaje de error indicando falta de conexión.
+Resultado obtenido: El posteo no se cancela ni se muestra mensaje claro de error, queda en estado incierto.</t>
+  </si>
+  <si>
+    <t>Comportamiento inconsistente al cargar posteos de perfil</t>
+  </si>
+  <si>
+    <t>1.Abrir app.
+2.Acceder al perfil.
+3.Seleccionar publicación.                                                                     4.Desplazarse verticalmente varias veces hacia arriba y abajo.</t>
+  </si>
+  <si>
+    <t>Resultado esperado: El desplazamiento debería ser fluido y las fotos deberían visualizarse completas y alineadas correctamente.
+Resultado obtenido: El desplazamiento presenta comportamiento inconsistente y algunas imágenes se muestran cortadas.</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/presentation/d/17pDPn_DlNzl3BlPgRcSaC-RDDuG4PUVFrM_S_Nqd6zY/edit?usp=sharing</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -59,7 +189,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -249,19 +379,109 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData/>
-  <drawing r:id="rId1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="55.42578125" customWidth="1"/>
+    <col min="2" max="2" width="71.85546875" customWidth="1"/>
+    <col min="3" max="3" width="47.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" tooltip="screenshot" xr:uid="{E71420A0-F7F4-4266-BEB2-0ED2FC0681C7}"/>
+    <hyperlink ref="E3:E4" r:id="rId2" display="https://docs.google.com/presentation/d/17pDPn_DlNzl3BlPgRcSaC-RDDuG4PUVFrM_S_Nqd6zY/edit?usp=sharing" xr:uid="{7BFD4FD8-53BF-4A65-B2CE-5C6C460EB26E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>